<commit_message>
updated homi user input
</commit_message>
<xml_diff>
--- a/YelpSummaryTop.xlsx
+++ b/YelpSummaryTop.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="104">
   <si>
     <t>category</t>
   </si>
@@ -40,12 +40,6 @@
     <t>15005</t>
   </si>
   <si>
-    <t>15006</t>
-  </si>
-  <si>
-    <t>15007</t>
-  </si>
-  <si>
     <t>15102</t>
   </si>
   <si>
@@ -55,15 +49,9 @@
     <t>15104</t>
   </si>
   <si>
-    <t>15015</t>
-  </si>
-  <si>
     <t>15017</t>
   </si>
   <si>
-    <t>15018</t>
-  </si>
-  <si>
     <t>15020</t>
   </si>
   <si>
@@ -82,9 +70,6 @@
     <t>15108</t>
   </si>
   <si>
-    <t>15028</t>
-  </si>
-  <si>
     <t>15030</t>
   </si>
   <si>
@@ -94,9 +79,6 @@
     <t>15031</t>
   </si>
   <si>
-    <t>15034</t>
-  </si>
-  <si>
     <t>15110</t>
   </si>
   <si>
@@ -121,21 +103,12 @@
     <t>15116</t>
   </si>
   <si>
-    <t>15047</t>
-  </si>
-  <si>
-    <t>15049</t>
-  </si>
-  <si>
     <t>15120</t>
   </si>
   <si>
     <t>15126</t>
   </si>
   <si>
-    <t>15051</t>
-  </si>
-  <si>
     <t>15642</t>
   </si>
   <si>
@@ -169,9 +142,6 @@
     <t>15146</t>
   </si>
   <si>
-    <t>15064</t>
-  </si>
-  <si>
     <t>15668</t>
   </si>
   <si>
@@ -190,9 +160,6 @@
     <t>15139</t>
   </si>
   <si>
-    <t>15140</t>
-  </si>
-  <si>
     <t>15201</t>
   </si>
   <si>
@@ -202,9 +169,6 @@
     <t>15203</t>
   </si>
   <si>
-    <t>15204</t>
-  </si>
-  <si>
     <t>15205</t>
   </si>
   <si>
@@ -305,18 +269,6 @@
   </si>
   <si>
     <t>15241</t>
-  </si>
-  <si>
-    <t>15243</t>
-  </si>
-  <si>
-    <t>15260</t>
-  </si>
-  <si>
-    <t>15290</t>
-  </si>
-  <si>
-    <t>15142</t>
   </si>
   <si>
     <t>15075</t>
@@ -731,7 +683,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E115"/>
+  <dimension ref="A1:E99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -759,16 +711,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C2">
         <v>10</v>
       </c>
       <c r="D2">
-        <v>3.959183673469388</v>
+        <v>3.957337883959045</v>
       </c>
       <c r="E2">
-        <v>29.4</v>
+        <v>29.3</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -776,16 +728,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3">
-        <v>4.2</v>
+        <v>4.199346405228758</v>
       </c>
       <c r="E3">
-        <v>19.375</v>
+        <v>21.85714285714286</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -793,7 +745,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -810,10 +762,16 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>3.681818181818182</v>
+      </c>
+      <c r="E5">
+        <v>37.71428571428572</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -821,10 +779,16 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>3.333333333333333</v>
+      </c>
+      <c r="E6">
+        <v>1.5</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -832,16 +796,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C7">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D7">
-        <v>3.614259597806216</v>
+        <v>4.231988472622478</v>
       </c>
       <c r="E7">
-        <v>36.46666666666667</v>
+        <v>86.75</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -849,16 +813,16 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="D8">
-        <v>3.75</v>
+        <v>3.298</v>
       </c>
       <c r="E8">
-        <v>1.333333333333333</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -866,16 +830,16 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>4.230659025787966</v>
+        <v>5</v>
       </c>
       <c r="E9">
-        <v>87.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -883,10 +847,16 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>4.119349005424954</v>
+      </c>
+      <c r="E10">
+        <v>110.6</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -894,16 +864,10 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C11">
-        <v>20</v>
-      </c>
-      <c r="D11">
-        <v>3.29452736318408</v>
-      </c>
-      <c r="E11">
-        <v>50.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -911,10 +875,16 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>3.213114754098361</v>
+      </c>
+      <c r="E12">
+        <v>12.2</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -922,16 +892,16 @@
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>3.137931034482758</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -939,16 +909,16 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C14">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D14">
-        <v>4.119241192411924</v>
+        <v>3.818345323741007</v>
       </c>
       <c r="E14">
-        <v>110.7</v>
+        <v>52.95238095238095</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -956,16 +926,16 @@
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="E15">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -973,16 +943,16 @@
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>3.213114754098361</v>
+        <v>3.5</v>
       </c>
       <c r="E16">
-        <v>12.2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -990,16 +960,16 @@
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17">
-        <v>3.137931034482758</v>
+        <v>3</v>
       </c>
       <c r="E17">
-        <v>14.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1007,16 +977,16 @@
         <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C18">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="D18">
-        <v>3.782945736434109</v>
+        <v>1</v>
       </c>
       <c r="E18">
-        <v>46.44</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1024,10 +994,16 @@
         <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>4.5</v>
+      </c>
+      <c r="E19">
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1035,7 +1011,7 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1044,7 +1020,7 @@
         <v>4</v>
       </c>
       <c r="E20">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1052,16 +1028,16 @@
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D21">
-        <v>3.5</v>
+        <v>3.605633802816901</v>
       </c>
       <c r="E21">
-        <v>4</v>
+        <v>11.83333333333333</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1069,16 +1045,16 @@
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22">
-        <v>3</v>
+        <v>3.166666666666667</v>
       </c>
       <c r="E22">
-        <v>8</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1086,10 +1062,16 @@
         <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="D23">
+        <v>3.405511811023622</v>
+      </c>
+      <c r="E23">
+        <v>29.30769230769231</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1097,16 +1079,16 @@
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E24">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1114,16 +1096,16 @@
         <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D25">
-        <v>4.5</v>
+        <v>3.922535211267606</v>
       </c>
       <c r="E25">
-        <v>14</v>
+        <v>47.33333333333334</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1131,16 +1113,16 @@
         <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D26">
-        <v>4</v>
+        <v>3.200308505949758</v>
       </c>
       <c r="E26">
-        <v>5</v>
+        <v>108.0476190476191</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1148,16 +1130,16 @@
         <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C27">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D27">
-        <v>3.605633802816901</v>
+        <v>4</v>
       </c>
       <c r="E27">
-        <v>11.83333333333333</v>
+        <v>21.66666666666667</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1165,16 +1147,16 @@
         <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D28">
-        <v>3.166666666666667</v>
+        <v>3.481641468682505</v>
       </c>
       <c r="E28">
-        <v>4.5</v>
+        <v>23.15</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1182,16 +1164,16 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C29">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D29">
-        <v>3.3828125</v>
+        <v>4</v>
       </c>
       <c r="E29">
-        <v>29.53846153846154</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1199,16 +1181,16 @@
         <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D30">
-        <v>4</v>
+        <v>3.701637666325486</v>
       </c>
       <c r="E30">
-        <v>6</v>
+        <v>81.41666666666667</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1216,16 +1198,16 @@
         <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C31">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D31">
-        <v>3.924028268551237</v>
+        <v>3.857142857142857</v>
       </c>
       <c r="E31">
-        <v>47.16666666666666</v>
+        <v>4.666666666666667</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1233,10 +1215,16 @@
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="D32">
+        <v>3.855828220858896</v>
+      </c>
+      <c r="E32">
+        <v>29.63636363636364</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1244,10 +1232,16 @@
         <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="D33">
+        <v>3.433962264150944</v>
+      </c>
+      <c r="E33">
+        <v>10.6</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1255,16 +1249,16 @@
         <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C34">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="D34">
-        <v>3.199517120280948</v>
+        <v>3.142857142857143</v>
       </c>
       <c r="E34">
-        <v>108.4761904761905</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1272,16 +1266,16 @@
         <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C35">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D35">
-        <v>3.977941176470588</v>
+        <v>4.25</v>
       </c>
       <c r="E35">
-        <v>13.6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1289,10 +1283,16 @@
         <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>3.409090909090909</v>
+      </c>
+      <c r="E36">
+        <v>5.5</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1300,16 +1300,16 @@
         <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C37">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D37">
-        <v>3.522435897435897</v>
+        <v>3.566666666666667</v>
       </c>
       <c r="E37">
-        <v>23.4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1317,16 +1317,16 @@
         <v>41</v>
       </c>
       <c r="B38" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C38">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="D38">
-        <v>4</v>
+        <v>3.559947643979057</v>
       </c>
       <c r="E38">
-        <v>14</v>
+        <v>54.57142857142857</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1334,16 +1334,16 @@
         <v>42</v>
       </c>
       <c r="B39" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C39">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D39">
-        <v>3.697662601626016</v>
+        <v>3.766260162601626</v>
       </c>
       <c r="E39">
-        <v>75.69230769230769</v>
+        <v>49.2</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1351,16 +1351,16 @@
         <v>43</v>
       </c>
       <c r="B40" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C40">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D40">
-        <v>3.857142857142857</v>
+        <v>3.397058823529412</v>
       </c>
       <c r="E40">
-        <v>4.666666666666667</v>
+        <v>13.6</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1368,16 +1368,16 @@
         <v>44</v>
       </c>
       <c r="B41" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C41">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D41">
-        <v>3.861027190332326</v>
+        <v>3.717821782178218</v>
       </c>
       <c r="E41">
-        <v>25.46153846153846</v>
+        <v>11.22222222222222</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1385,16 +1385,16 @@
         <v>45</v>
       </c>
       <c r="B42" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C42">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D42">
-        <v>3.447368421052631</v>
+        <v>3.214788732394366</v>
       </c>
       <c r="E42">
-        <v>12.66666666666667</v>
+        <v>15.77777777777778</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1402,16 +1402,16 @@
         <v>46</v>
       </c>
       <c r="B43" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C43">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D43">
-        <v>2.875</v>
+        <v>3.927480916030534</v>
       </c>
       <c r="E43">
-        <v>3.2</v>
+        <v>16.375</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1419,16 +1419,16 @@
         <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C44">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D44">
-        <v>4.25</v>
+        <v>3.605603448275862</v>
       </c>
       <c r="E44">
-        <v>2</v>
+        <v>51.55555555555556</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1436,16 +1436,16 @@
         <v>48</v>
       </c>
       <c r="B45" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C45">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="D45">
-        <v>3.409090909090909</v>
+        <v>3.760378983634797</v>
       </c>
       <c r="E45">
-        <v>5.5</v>
+        <v>207.3214285714286</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1453,16 +1453,16 @@
         <v>49</v>
       </c>
       <c r="B46" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C46">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D46">
-        <v>3.566666666666667</v>
+        <v>3.847545219638243</v>
       </c>
       <c r="E46">
-        <v>6</v>
+        <v>38.7</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1470,16 +1470,16 @@
         <v>50</v>
       </c>
       <c r="B47" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C47">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D47">
-        <v>3.558485639686684</v>
+        <v>3.909684116861931</v>
       </c>
       <c r="E47">
-        <v>53.19444444444444</v>
+        <v>149.8444444444444</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1487,10 +1487,16 @@
         <v>51</v>
       </c>
       <c r="B48" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="D48">
+        <v>3.555164835164835</v>
+      </c>
+      <c r="E48">
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1498,16 +1504,16 @@
         <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C49">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="D49">
-        <v>3.76554054054054</v>
+        <v>3.997177267595032</v>
       </c>
       <c r="E49">
-        <v>49.33333333333334</v>
+        <v>204.3846153846154</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1515,16 +1521,16 @@
         <v>53</v>
       </c>
       <c r="B50" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C50">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D50">
-        <v>3.414285714285714</v>
+        <v>3.977040816326531</v>
       </c>
       <c r="E50">
-        <v>10</v>
+        <v>65.33333333333333</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1532,16 +1538,16 @@
         <v>54</v>
       </c>
       <c r="B51" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C51">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="D51">
-        <v>3.688073394495413</v>
+        <v>4.486607142857143</v>
       </c>
       <c r="E51">
-        <v>11.47368421052632</v>
+        <v>37.33333333333334</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1549,16 +1555,16 @@
         <v>55</v>
       </c>
       <c r="B52" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C52">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D52">
-        <v>3.269230769230769</v>
+        <v>3.87246963562753</v>
       </c>
       <c r="E52">
-        <v>15.88888888888889</v>
+        <v>35.28571428571428</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1566,16 +1572,16 @@
         <v>56</v>
       </c>
       <c r="B53" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C53">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D53">
-        <v>3.932330827067669</v>
+        <v>3.714285714285714</v>
       </c>
       <c r="E53">
-        <v>14.77777777777778</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1583,16 +1589,16 @@
         <v>57</v>
       </c>
       <c r="B54" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C54">
         <v>9</v>
       </c>
       <c r="D54">
-        <v>3.605603448275862</v>
+        <v>4.121104185218166</v>
       </c>
       <c r="E54">
-        <v>51.55555555555556</v>
+        <v>249.5555555555555</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1600,10 +1606,16 @@
         <v>58</v>
       </c>
       <c r="B55" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="D55">
+        <v>3.832309582309582</v>
+      </c>
+      <c r="E55">
+        <v>58.14285714285715</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1611,16 +1623,16 @@
         <v>59</v>
       </c>
       <c r="B56" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C56">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D56">
-        <v>3.779331457885156</v>
+        <v>3.742219215155616</v>
       </c>
       <c r="E56">
-        <v>201.4333333333333</v>
+        <v>131.3777777777778</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1628,16 +1640,16 @@
         <v>60</v>
       </c>
       <c r="B57" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C57">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D57">
-        <v>3.847096774193548</v>
+        <v>5</v>
       </c>
       <c r="E57">
-        <v>38.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1645,16 +1657,16 @@
         <v>61</v>
       </c>
       <c r="B58" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C58">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="D58">
-        <v>3.93231102850062</v>
+        <v>3.52212389380531</v>
       </c>
       <c r="E58">
-        <v>137.3617021276596</v>
+        <v>48.42857142857143</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1662,10 +1674,16 @@
         <v>62</v>
       </c>
       <c r="B59" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="D59">
+        <v>3.642351660315732</v>
+      </c>
+      <c r="E59">
+        <v>83.5</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1673,16 +1691,16 @@
         <v>63</v>
       </c>
       <c r="B60" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C60">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D60">
-        <v>3.636545293072824</v>
+        <v>3.690427698574338</v>
       </c>
       <c r="E60">
-        <v>86.61538461538461</v>
+        <v>158.8529411764706</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1690,16 +1708,16 @@
         <v>64</v>
       </c>
       <c r="B61" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C61">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D61">
-        <v>3.992704588707972</v>
+        <v>4.124896608767576</v>
       </c>
       <c r="E61">
-        <v>189.16</v>
+        <v>100.75</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -1707,16 +1725,16 @@
         <v>65</v>
       </c>
       <c r="B62" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C62">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="D62">
-        <v>3.977040816326531</v>
+        <v>3.909978880675818</v>
       </c>
       <c r="E62">
-        <v>65.33333333333333</v>
+        <v>94.7</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1724,16 +1742,16 @@
         <v>66</v>
       </c>
       <c r="B63" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C63">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D63">
-        <v>4.486607142857143</v>
+        <v>3.584249084249084</v>
       </c>
       <c r="E63">
-        <v>37.33333333333334</v>
+        <v>45.5</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -1741,16 +1759,16 @@
         <v>67</v>
       </c>
       <c r="B64" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C64">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D64">
-        <v>3.904833836858006</v>
+        <v>4.004237288135593</v>
       </c>
       <c r="E64">
-        <v>41.375</v>
+        <v>29.5</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -1758,16 +1776,16 @@
         <v>68</v>
       </c>
       <c r="B65" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C65">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="D65">
-        <v>4.245901639344262</v>
+        <v>4.118747308189257</v>
       </c>
       <c r="E65">
-        <v>30.5</v>
+        <v>285.140350877193</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -1775,16 +1793,16 @@
         <v>69</v>
       </c>
       <c r="B66" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C66">
         <v>7</v>
       </c>
       <c r="D66">
-        <v>4.150696378830084</v>
+        <v>4.012422360248447</v>
       </c>
       <c r="E66">
-        <v>256.4285714285714</v>
+        <v>23</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -1792,16 +1810,16 @@
         <v>70</v>
       </c>
       <c r="B67" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C67">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D67">
-        <v>3.707638279192274</v>
+        <v>3.869124683366169</v>
       </c>
       <c r="E67">
-        <v>54.23809523809524</v>
+        <v>122.5172413793103</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -1809,16 +1827,16 @@
         <v>71</v>
       </c>
       <c r="B68" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C68">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="D68">
-        <v>3.721441266763613</v>
+        <v>3.678571428571428</v>
       </c>
       <c r="E68">
-        <v>123.78</v>
+        <v>35</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -1826,16 +1844,16 @@
         <v>72</v>
       </c>
       <c r="B69" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C69">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D69">
-        <v>5</v>
+        <v>4.238738738738738</v>
       </c>
       <c r="E69">
-        <v>1</v>
+        <v>41.625</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -1843,16 +1861,16 @@
         <v>73</v>
       </c>
       <c r="B70" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C70">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D70">
-        <v>3.514705882352941</v>
+        <v>3.939759036144578</v>
       </c>
       <c r="E70">
-        <v>42.5</v>
+        <v>23.71428571428572</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -1860,16 +1878,16 @@
         <v>74</v>
       </c>
       <c r="B71" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C71">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D71">
-        <v>3.629839958699019</v>
+        <v>4.009595959595959</v>
       </c>
       <c r="E71">
-        <v>77.48</v>
+        <v>123.75</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -1877,16 +1895,16 @@
         <v>75</v>
       </c>
       <c r="B72" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C72">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="D72">
-        <v>3.665558019216556</v>
+        <v>4.5</v>
       </c>
       <c r="E72">
-        <v>159.1764705882353</v>
+        <v>54.75</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -1894,16 +1912,16 @@
         <v>76</v>
       </c>
       <c r="B73" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C73">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D73">
-        <v>4.124380165289256</v>
+        <v>3.707438281500481</v>
       </c>
       <c r="E73">
-        <v>100.8333333333333</v>
+        <v>135.6086956521739</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -1911,16 +1929,16 @@
         <v>77</v>
       </c>
       <c r="B74" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C74">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="D74">
-        <v>3.905260332796565</v>
+        <v>4.102424242424243</v>
       </c>
       <c r="E74">
-        <v>74.52</v>
+        <v>165</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -1928,16 +1946,16 @@
         <v>78</v>
       </c>
       <c r="B75" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C75">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D75">
-        <v>3.578583765112263</v>
+        <v>3.548387096774194</v>
       </c>
       <c r="E75">
-        <v>44.53846153846154</v>
+        <v>54.25</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -1945,16 +1963,16 @@
         <v>79</v>
       </c>
       <c r="B76" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C76">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D76">
-        <v>3.858695652173913</v>
+        <v>3.943306010928962</v>
       </c>
       <c r="E76">
-        <v>27.6</v>
+        <v>52.28571428571428</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -1962,16 +1980,16 @@
         <v>80</v>
       </c>
       <c r="B77" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C77">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="D77">
-        <v>4.105998576005696</v>
+        <v>3.421862011637573</v>
       </c>
       <c r="E77">
-        <v>263.34375</v>
+        <v>50.125</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -1979,16 +1997,16 @@
         <v>81</v>
       </c>
       <c r="B78" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C78">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="D78">
-        <v>4.003086419753086</v>
+        <v>3.576799485861183</v>
       </c>
       <c r="E78">
-        <v>23.14285714285714</v>
+        <v>75.90243902439025</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -1996,16 +2014,16 @@
         <v>82</v>
       </c>
       <c r="B79" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C79">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D79">
-        <v>3.909831756046267</v>
+        <v>3.654159132007233</v>
       </c>
       <c r="E79">
-        <v>126.8</v>
+        <v>65.05882352941177</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -2013,16 +2031,16 @@
         <v>83</v>
       </c>
       <c r="B80" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C80">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D80">
-        <v>3.678571428571428</v>
+        <v>3.791907514450867</v>
       </c>
       <c r="E80">
-        <v>35</v>
+        <v>21.625</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -2030,16 +2048,16 @@
         <v>84</v>
       </c>
       <c r="B81" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C81">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D81">
-        <v>4.232035928143713</v>
+        <v>3.183011049723757</v>
       </c>
       <c r="E81">
-        <v>41.75</v>
+        <v>51.71428571428572</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -2047,16 +2065,16 @@
         <v>85</v>
       </c>
       <c r="B82" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C82">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D82">
-        <v>3.940476190476191</v>
+        <v>4.5</v>
       </c>
       <c r="E82">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -2064,16 +2082,16 @@
         <v>86</v>
       </c>
       <c r="B83" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C83">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D83">
-        <v>4.009329299041855</v>
+        <v>4.569767441860465</v>
       </c>
       <c r="E83">
-        <v>123.9375</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -2081,16 +2099,16 @@
         <v>87</v>
       </c>
       <c r="B84" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C84">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D84">
-        <v>4.5</v>
+        <v>3.55</v>
       </c>
       <c r="E84">
-        <v>54.75</v>
+        <v>10</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -2098,16 +2116,16 @@
         <v>88</v>
       </c>
       <c r="B85" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C85">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D85">
-        <v>3.745762711864407</v>
+        <v>3.611111111111111</v>
       </c>
       <c r="E85">
-        <v>143.6521739130435</v>
+        <v>49.5</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -2115,16 +2133,16 @@
         <v>89</v>
       </c>
       <c r="B86" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C86">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D86">
-        <v>4.102905569007264</v>
+        <v>3.513986013986014</v>
       </c>
       <c r="E86">
-        <v>165.2</v>
+        <v>35.75</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -2132,16 +2150,16 @@
         <v>90</v>
       </c>
       <c r="B87" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C87">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="D87">
-        <v>3.55166475315729</v>
+        <v>4.322222222222222</v>
       </c>
       <c r="E87">
-        <v>51.23529411764706</v>
+        <v>45</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -2149,16 +2167,16 @@
         <v>91</v>
       </c>
       <c r="B88" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C88">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D88">
-        <v>3.880050505050505</v>
+        <v>4.5</v>
       </c>
       <c r="E88">
-        <v>46.58823529411764</v>
+        <v>7</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -2166,16 +2184,16 @@
         <v>92</v>
       </c>
       <c r="B89" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C89">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D89">
-        <v>3.435456110154905</v>
+        <v>3.08273381294964</v>
       </c>
       <c r="E89">
-        <v>50.52173913043478</v>
+        <v>19.85714285714286</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -2183,16 +2201,16 @@
         <v>93</v>
       </c>
       <c r="B90" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C90">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="D90">
-        <v>3.558072009291521</v>
+        <v>4.5</v>
       </c>
       <c r="E90">
-        <v>74.8695652173913</v>
+        <v>7</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -2200,16 +2218,16 @@
         <v>94</v>
       </c>
       <c r="B91" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C91">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="D91">
-        <v>3.55</v>
+        <v>4.25984251968504</v>
       </c>
       <c r="E91">
-        <v>56.95652173913044</v>
+        <v>31.75</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -2217,16 +2235,16 @@
         <v>95</v>
       </c>
       <c r="B92" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C92">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D92">
-        <v>3.790697674418605</v>
+        <v>2.5</v>
       </c>
       <c r="E92">
-        <v>21.5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -2234,16 +2252,16 @@
         <v>96</v>
       </c>
       <c r="B93" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C93">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D93">
-        <v>3.178523489932886</v>
+        <v>4</v>
       </c>
       <c r="E93">
-        <v>53.21428571428572</v>
+        <v>26</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -2251,10 +2269,16 @@
         <v>97</v>
       </c>
       <c r="B94" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C94">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="D94">
+        <v>4.119834710743802</v>
+      </c>
+      <c r="E94">
+        <v>90.75</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -2262,10 +2286,16 @@
         <v>98</v>
       </c>
       <c r="B95" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C95">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="D95">
+        <v>4.5</v>
+      </c>
+      <c r="E95">
+        <v>3</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -2273,10 +2303,16 @@
         <v>99</v>
       </c>
       <c r="B96" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C96">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="D96">
+        <v>3.112094395280236</v>
+      </c>
+      <c r="E96">
+        <v>26.07692307692308</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -2284,10 +2320,16 @@
         <v>100</v>
       </c>
       <c r="B97" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C97">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="D97">
+        <v>3.620481927710844</v>
+      </c>
+      <c r="E97">
+        <v>41.5</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -2295,16 +2337,16 @@
         <v>101</v>
       </c>
       <c r="B98" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C98">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D98">
-        <v>4.5</v>
+        <v>3.503894839337877</v>
       </c>
       <c r="E98">
-        <v>15</v>
+        <v>68.46666666666667</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -2312,287 +2354,15 @@
         <v>102</v>
       </c>
       <c r="B99" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C99">
         <v>2</v>
       </c>
       <c r="D99">
-        <v>4.569767441860465</v>
+        <v>4.078947368421052</v>
       </c>
       <c r="E99">
-        <v>21.5</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5">
-      <c r="A100" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B100" t="s">
-        <v>119</v>
-      </c>
-      <c r="C100">
-        <v>8</v>
-      </c>
-      <c r="D100">
-        <v>3.55</v>
-      </c>
-      <c r="E100">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5">
-      <c r="A101" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B101" t="s">
-        <v>119</v>
-      </c>
-      <c r="C101">
-        <v>13</v>
-      </c>
-      <c r="D101">
-        <v>3.610552763819095</v>
-      </c>
-      <c r="E101">
-        <v>45.92307692307692</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5">
-      <c r="A102" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B102" t="s">
-        <v>119</v>
-      </c>
-      <c r="C102">
-        <v>4</v>
-      </c>
-      <c r="D102">
-        <v>3.506896551724138</v>
-      </c>
-      <c r="E102">
-        <v>36.25</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5">
-      <c r="A103" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B103" t="s">
-        <v>119</v>
-      </c>
-      <c r="C103">
-        <v>4</v>
-      </c>
-      <c r="D103">
-        <v>4.323204419889502</v>
-      </c>
-      <c r="E103">
-        <v>45.25</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5">
-      <c r="A104" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B104" t="s">
-        <v>119</v>
-      </c>
-      <c r="C104">
-        <v>1</v>
-      </c>
-      <c r="D104">
-        <v>4.5</v>
-      </c>
-      <c r="E104">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5">
-      <c r="A105" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B105" t="s">
-        <v>119</v>
-      </c>
-      <c r="C105">
-        <v>15</v>
-      </c>
-      <c r="D105">
-        <v>3.127118644067797</v>
-      </c>
-      <c r="E105">
-        <v>19.66666666666667</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5">
-      <c r="A106" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B106" t="s">
-        <v>119</v>
-      </c>
-      <c r="C106">
-        <v>1</v>
-      </c>
-      <c r="D106">
-        <v>4.5</v>
-      </c>
-      <c r="E106">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5">
-      <c r="A107" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B107" t="s">
-        <v>119</v>
-      </c>
-      <c r="C107">
-        <v>4</v>
-      </c>
-      <c r="D107">
-        <v>4.25984251968504</v>
-      </c>
-      <c r="E107">
-        <v>31.75</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5">
-      <c r="A108" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B108" t="s">
-        <v>119</v>
-      </c>
-      <c r="C108">
-        <v>1</v>
-      </c>
-      <c r="D108">
-        <v>2.5</v>
-      </c>
-      <c r="E108">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5">
-      <c r="A109" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B109" t="s">
-        <v>119</v>
-      </c>
-      <c r="C109">
-        <v>3</v>
-      </c>
-      <c r="D109">
-        <v>4</v>
-      </c>
-      <c r="E109">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5">
-      <c r="A110" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B110" t="s">
-        <v>119</v>
-      </c>
-      <c r="C110">
-        <v>5</v>
-      </c>
-      <c r="D110">
-        <v>4.1146408839779</v>
-      </c>
-      <c r="E110">
-        <v>72.40000000000001</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5">
-      <c r="A111" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B111" t="s">
-        <v>119</v>
-      </c>
-      <c r="C111">
-        <v>2</v>
-      </c>
-      <c r="D111">
-        <v>4.5</v>
-      </c>
-      <c r="E111">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5">
-      <c r="A112" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B112" t="s">
-        <v>119</v>
-      </c>
-      <c r="C112">
-        <v>14</v>
-      </c>
-      <c r="D112">
-        <v>3.117302052785924</v>
-      </c>
-      <c r="E112">
-        <v>24.35714285714286</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5">
-      <c r="A113" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B113" t="s">
-        <v>119</v>
-      </c>
-      <c r="C113">
-        <v>2</v>
-      </c>
-      <c r="D113">
-        <v>3.620481927710844</v>
-      </c>
-      <c r="E113">
-        <v>41.5</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5">
-      <c r="A114" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B114" t="s">
-        <v>119</v>
-      </c>
-      <c r="C114">
-        <v>15</v>
-      </c>
-      <c r="D114">
-        <v>3.503894839337877</v>
-      </c>
-      <c r="E114">
-        <v>68.46666666666667</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5">
-      <c r="A115" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B115" t="s">
-        <v>119</v>
-      </c>
-      <c r="C115">
-        <v>2</v>
-      </c>
-      <c r="D115">
-        <v>4.078947368421052</v>
-      </c>
-      <c r="E115">
         <v>9.5</v>
       </c>
     </row>

</xml_diff>